<commit_message>
Able to pass parameter_count back to view controller; fetching the POST data and generating conditions
</commit_message>
<xml_diff>
--- a/media/vlz_report.xlsx
+++ b/media/vlz_report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rajn/PycharmProjects/TaaraMail/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38856BD1-F3F4-1646-87DD-74248AAE30DC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C4BFBA-0996-E44F-90A5-A4431919B2D7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{720CE2AB-B664-744E-8AEB-29CC10E0D1AA}"/>
   </bookViews>
@@ -537,7 +537,7 @@
   <dimension ref="A1:Y4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>